<commit_message>
[376942] Third-Party Tool Extensions not handled correctly https://bugs.eclipse.org/bugs/show_bug.cgi?id=376942
added more test cases and fixed a bug that occurred in case of multiple
non empty ReqIFToolExtensions were used in the model
</commit_message>
<xml_diff>
--- a/org.eclipse.rmf.reqif10.tests/doc/Serialization.xlsx
+++ b/org.eclipse.rmf.reqif10.tests/doc/Serialization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24260" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="26920" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="XML Save Feature Kinds" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,12 @@
     <sheet name="ExtendedMetaData Content Kind" sheetId="3" r:id="rId3"/>
     <sheet name="Wildcard Processing" sheetId="4" r:id="rId4"/>
     <sheet name="TestSpec TC0001000" sheetId="5" r:id="rId5"/>
+    <sheet name="Blatt1" sheetId="6" r:id="rId6"/>
+    <sheet name="TestSpec TC0004001" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'TestSpec TC0001000'!$A$4:$H$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'TestSpec TC0004001'!$A$4:$I$13</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="146">
   <si>
     <t>ID</t>
   </si>
@@ -398,6 +401,72 @@
   </si>
   <si>
     <t>ReqIFHeader.title</t>
+  </si>
+  <si>
+    <t>NodeWithReferences.singleUnsetDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithReferences.singleSetNotDefaultValue</t>
+  </si>
+  <si>
+    <t>unsetable</t>
+  </si>
+  <si>
+    <t>NodeWithReferences.manyUnssetDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithReferences.manySetNotDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithAttributes.singleUnsetDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithAttributes.singleSetNotDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithAttributes.manyUnssetDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithAttributes.manySetNotDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithAttributes.manySetDefaultValue</t>
+  </si>
+  <si>
+    <t>NodeWithReferencesUnsetable.singleUnsetDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithReferencesUnsetable.singleSetNotDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithReferencesUnsetable.singleSetDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithReferencesUnsetable.manyUnssetDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithReferencesUnsetable.manySetNotDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithReferencesUnsetable.manySetDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithAttributesUnsetable.singleUnsetDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithAttributesUnsetable.singleSetNotDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithAttributesUnsetable.singleSetDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithAttributesUnsetable.manyUnssetDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithAttributesUnsetable.manySetNotDefaultValueUnsetable</t>
+  </si>
+  <si>
+    <t>NodeWithAttributesUnsetable.manySetDefaultValueUnsetable</t>
   </si>
 </sst>
 </file>
@@ -446,8 +515,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -500,7 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="69">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -524,6 +615,17 @@
     <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -547,6 +649,17 @@
     <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1954,7 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -2381,4 +2494,907 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="65.6640625" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" t="s">
+        <v>111</v>
+      </c>
+      <c r="H31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A4:I13"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>